<commit_message>
added the save to excel part
</commit_message>
<xml_diff>
--- a/device_report.xlsx
+++ b/device_report.xlsx
@@ -1,73 +1,40 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21929"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="Z:\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C9CFCF78-05BD-4E86-962C-1F98BDA63BED}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2304" yWindow="2304" windowWidth="17280" windowHeight="9024" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView activeTab="0" autoFilterDateGrouping="1" firstSheet="0" minimized="0" showHorizontalScroll="1" showSheetTabs="1" showVerticalScroll="1" tabRatio="600" visibility="visible" windowHeight="11325" windowWidth="21600" xWindow="1350" yWindow="1350"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet" sheetId="1" r:id="rId1"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheet" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <definedNames/>
+  <calcPr calcId="0" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
-<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
-  <si>
-    <t>ip address</t>
-  </si>
-  <si>
-    <t>version</t>
-  </si>
-  <si>
-    <t xml:space="preserve">vc count </t>
-  </si>
-  <si>
-    <t>master RE memory utilization</t>
-  </si>
-  <si>
-    <t>master RE cpu utilization</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ntp ip </t>
-  </si>
-  <si>
-    <t>ntp status</t>
-  </si>
-  <si>
-    <t>all vc present</t>
-  </si>
-  <si>
-    <t>model</t>
-  </si>
-  <si>
-    <t>host name</t>
-  </si>
-</sst>
-</file>
-
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <numFmts count="0"/>
+  <fonts count="2">
     <font>
-      <sz val="11"/>
-      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
+      <color theme="1"/>
+      <sz val="11"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <color rgb="FFFF0000"/>
+      <sz val="11"/>
       <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="3">
     <fill>
-      <patternFill patternType="none"/>
+      <patternFill/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
@@ -89,25 +56,17 @@
     </border>
   </borders>
   <cellStyleXfs count="1">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+  <cellXfs count="3">
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf borderId="0" fillId="2" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle builtinId="0" name="Normal" xfId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
-    </ext>
-  </extLst>
+  <tableStyles count="0" defaultPivotStyle="PivotStyleLight16" defaultTableStyle="TableStyleMedium9"/>
 </styleSheet>
 </file>
 
@@ -395,55 +354,181 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:J1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:H4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J6" sqref="J6"/>
+      <selection activeCell="A2" sqref="A2:A4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" width="11.21875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="9.109375" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="11.6640625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="24.77734375" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="20.77734375" bestFit="1" customWidth="1"/>
+    <col bestFit="1" customWidth="1" max="1" min="1" width="11.21875"/>
+    <col bestFit="1" customWidth="1" max="4" min="4" width="9.109375"/>
+    <col bestFit="1" customWidth="1" max="6" min="6" width="11.6640625"/>
+    <col bestFit="1" customWidth="1" max="7" min="7" width="20.77734375"/>
+    <col bestFit="1" customWidth="1" max="8" min="8" width="24.77734375"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A1" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="B1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="D1" t="s">
-        <v>0</v>
-      </c>
-      <c r="E1" t="s">
-        <v>2</v>
-      </c>
-      <c r="F1" t="s">
-        <v>7</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="H1" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="I1" t="s">
-        <v>5</v>
-      </c>
-      <c r="J1" t="s">
-        <v>6</v>
+    <row r="1">
+      <c r="A1" s="1" t="inlineStr">
+        <is>
+          <t>host name</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>version</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
+          <t>model</t>
+        </is>
+      </c>
+      <c r="D1" t="inlineStr">
+        <is>
+          <t>ip address</t>
+        </is>
+      </c>
+      <c r="E1" t="inlineStr">
+        <is>
+          <t xml:space="preserve">vc count </t>
+        </is>
+      </c>
+      <c r="F1" s="2" t="inlineStr">
+        <is>
+          <t>all vc present</t>
+        </is>
+      </c>
+      <c r="G1" s="1" t="inlineStr">
+        <is>
+          <t>master RE cpu utilization</t>
+        </is>
+      </c>
+      <c r="H1" s="1" t="inlineStr">
+        <is>
+          <t>master RE memory utilization</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>floor7_sw_lab</t>
+        </is>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>JUNOS Base OS boot [12.3R12.4]</t>
+        </is>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>ex3300-24p</t>
+        </is>
+      </c>
+      <c r="D2" t="inlineStr">
+        <is>
+          <t>10.9.106.30/23</t>
+        </is>
+      </c>
+      <c r="E2" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="G2" t="inlineStr">
+        <is>
+          <t>4</t>
+        </is>
+      </c>
+      <c r="H2" t="inlineStr">
+        <is>
+          <t>34</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>PTSW2_Floor7</t>
+        </is>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>JUNOS Base OS boot [12.3R12.4]</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>ex3300-48p</t>
+        </is>
+      </c>
+      <c r="D3" t="inlineStr">
+        <is>
+          <t>10.9.106.38/23</t>
+        </is>
+      </c>
+      <c r="E3" t="inlineStr">
+        <is>
+          <t>4</t>
+        </is>
+      </c>
+      <c r="G3" t="inlineStr">
+        <is>
+          <t>72</t>
+        </is>
+      </c>
+      <c r="H3" t="inlineStr">
+        <is>
+          <t>38</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>PTSW1_Floor7</t>
+        </is>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>JUNOS Base OS boot [12.3R12.4]</t>
+        </is>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>ex3300-48p</t>
+        </is>
+      </c>
+      <c r="D4" t="inlineStr">
+        <is>
+          <t>10.9.106.37/23</t>
+        </is>
+      </c>
+      <c r="E4" t="inlineStr">
+        <is>
+          <t>4</t>
+        </is>
+      </c>
+      <c r="G4" t="inlineStr">
+        <is>
+          <t>66</t>
+        </is>
+      </c>
+      <c r="H4" t="inlineStr">
+        <is>
+          <t>39</t>
+        </is>
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
+  <pageSetup horizontalDpi="180" orientation="landscape" paperSize="261" verticalDpi="180"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
move all gathered facts into dictonary
</commit_message>
<xml_diff>
--- a/device_report.xlsx
+++ b/device_report.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <bookViews>
-    <workbookView activeTab="0" autoFilterDateGrouping="1" firstSheet="0" minimized="0" showHorizontalScroll="1" showSheetTabs="1" showVerticalScroll="1" tabRatio="600" visibility="visible" windowHeight="11325" windowWidth="21600" xWindow="1350" yWindow="1350"/>
+    <workbookView activeTab="0" autoFilterDateGrouping="1" firstSheet="0" minimized="0" showHorizontalScroll="1" showSheetTabs="1" showVerticalScroll="1" tabRatio="600" visibility="visible" windowHeight="11325" windowWidth="21600" xWindow="5655" yWindow="2730"/>
   </bookViews>
   <sheets>
     <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheet" sheetId="1" state="visible" r:id="rId1"/>
@@ -359,19 +359,19 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:H4"/>
+  <dimension ref="A1:H22"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:A4"/>
+      <selection activeCell="H9" sqref="H9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="14.4"/>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <cols>
-    <col bestFit="1" customWidth="1" max="1" min="1" width="11.21875"/>
-    <col bestFit="1" customWidth="1" max="4" min="4" width="9.109375"/>
-    <col bestFit="1" customWidth="1" max="6" min="6" width="11.6640625"/>
-    <col bestFit="1" customWidth="1" max="7" min="7" width="20.77734375"/>
-    <col bestFit="1" customWidth="1" max="8" min="8" width="24.77734375"/>
+    <col bestFit="1" customWidth="1" max="1" min="1" width="11.28515625"/>
+    <col bestFit="1" customWidth="1" max="4" min="4" width="9.140625"/>
+    <col bestFit="1" customWidth="1" max="6" min="6" width="11.7109375"/>
+    <col bestFit="1" customWidth="1" max="7" min="7" width="20.7109375"/>
+    <col bestFit="1" customWidth="1" max="8" min="8" width="24.7109375"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -444,7 +444,7 @@
       </c>
       <c r="G2" t="inlineStr">
         <is>
-          <t>4</t>
+          <t>6</t>
         </is>
       </c>
       <c r="H2" t="inlineStr">
@@ -481,7 +481,7 @@
       </c>
       <c r="G3" t="inlineStr">
         <is>
-          <t>72</t>
+          <t>71</t>
         </is>
       </c>
       <c r="H3" t="inlineStr">
@@ -518,12 +518,678 @@
       </c>
       <c r="G4" t="inlineStr">
         <is>
-          <t>66</t>
+          <t>71</t>
         </is>
       </c>
       <c r="H4" t="inlineStr">
         <is>
           <t>39</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>floor7_sw_lab</t>
+        </is>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>JUNOS Base OS boot [12.3R12.4]</t>
+        </is>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>ex3300-24p</t>
+        </is>
+      </c>
+      <c r="D5" t="inlineStr">
+        <is>
+          <t>10.9.106.30/23</t>
+        </is>
+      </c>
+      <c r="E5" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="G5" t="inlineStr">
+        <is>
+          <t>4</t>
+        </is>
+      </c>
+      <c r="H5" t="inlineStr">
+        <is>
+          <t>34</t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>PTSW2_Floor7</t>
+        </is>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>JUNOS Base OS boot [12.3R12.4]</t>
+        </is>
+      </c>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>ex3300-48p</t>
+        </is>
+      </c>
+      <c r="D6" t="inlineStr">
+        <is>
+          <t>10.9.106.38/23</t>
+        </is>
+      </c>
+      <c r="E6" t="inlineStr">
+        <is>
+          <t>4</t>
+        </is>
+      </c>
+      <c r="G6" t="inlineStr">
+        <is>
+          <t>73</t>
+        </is>
+      </c>
+      <c r="H6" t="inlineStr">
+        <is>
+          <t>38</t>
+        </is>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>PTSW1_Floor7</t>
+        </is>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>JUNOS Base OS boot [12.3R12.4]</t>
+        </is>
+      </c>
+      <c r="C7" t="inlineStr">
+        <is>
+          <t>ex3300-48p</t>
+        </is>
+      </c>
+      <c r="D7" t="inlineStr">
+        <is>
+          <t>10.9.106.37/23</t>
+        </is>
+      </c>
+      <c r="E7" t="inlineStr">
+        <is>
+          <t>4</t>
+        </is>
+      </c>
+      <c r="G7" t="inlineStr">
+        <is>
+          <t>69</t>
+        </is>
+      </c>
+      <c r="H7" t="inlineStr">
+        <is>
+          <t>39</t>
+        </is>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>floor7_sw_lab</t>
+        </is>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>JUNOS Base OS boot [12.3R12.4]</t>
+        </is>
+      </c>
+      <c r="C8" t="inlineStr">
+        <is>
+          <t>ex3300-24p</t>
+        </is>
+      </c>
+      <c r="D8" t="inlineStr">
+        <is>
+          <t>10.9.106.30/23</t>
+        </is>
+      </c>
+      <c r="E8" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="G8" t="inlineStr">
+        <is>
+          <t>4</t>
+        </is>
+      </c>
+      <c r="H8" t="inlineStr">
+        <is>
+          <t>34</t>
+        </is>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>PTSW2_Floor7</t>
+        </is>
+      </c>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>JUNOS Base OS boot [12.3R12.4]</t>
+        </is>
+      </c>
+      <c r="C9" t="inlineStr">
+        <is>
+          <t>ex3300-48p</t>
+        </is>
+      </c>
+      <c r="D9" t="inlineStr">
+        <is>
+          <t>10.9.106.38/23</t>
+        </is>
+      </c>
+      <c r="E9" t="inlineStr">
+        <is>
+          <t>4</t>
+        </is>
+      </c>
+      <c r="G9" t="inlineStr">
+        <is>
+          <t>81</t>
+        </is>
+      </c>
+      <c r="H9" t="inlineStr">
+        <is>
+          <t>38</t>
+        </is>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="inlineStr">
+        <is>
+          <t>PTSW1_Floor7</t>
+        </is>
+      </c>
+      <c r="B10" t="inlineStr">
+        <is>
+          <t>JUNOS Base OS boot [12.3R12.4]</t>
+        </is>
+      </c>
+      <c r="C10" t="inlineStr">
+        <is>
+          <t>ex3300-48p</t>
+        </is>
+      </c>
+      <c r="D10" t="inlineStr">
+        <is>
+          <t>10.9.106.37/23</t>
+        </is>
+      </c>
+      <c r="E10" t="inlineStr">
+        <is>
+          <t>4</t>
+        </is>
+      </c>
+      <c r="G10" t="inlineStr">
+        <is>
+          <t>69</t>
+        </is>
+      </c>
+      <c r="H10" t="inlineStr">
+        <is>
+          <t>39</t>
+        </is>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="inlineStr">
+        <is>
+          <t>floor7_sw_lab</t>
+        </is>
+      </c>
+      <c r="B11" t="inlineStr">
+        <is>
+          <t>JUNOS Base OS boot [12.3R12.4]</t>
+        </is>
+      </c>
+      <c r="C11" t="inlineStr">
+        <is>
+          <t>ex3300-24p</t>
+        </is>
+      </c>
+      <c r="D11" t="inlineStr">
+        <is>
+          <t>10.9.106.30/23</t>
+        </is>
+      </c>
+      <c r="E11" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="G11" t="inlineStr">
+        <is>
+          <t>4</t>
+        </is>
+      </c>
+      <c r="H11" t="inlineStr">
+        <is>
+          <t>34</t>
+        </is>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="inlineStr">
+        <is>
+          <t>PTSW2_Floor7</t>
+        </is>
+      </c>
+      <c r="B12" t="inlineStr">
+        <is>
+          <t>JUNOS Base OS boot [12.3R12.4]</t>
+        </is>
+      </c>
+      <c r="C12" t="inlineStr">
+        <is>
+          <t>ex3300-48p</t>
+        </is>
+      </c>
+      <c r="D12" t="inlineStr">
+        <is>
+          <t>10.9.106.38/23</t>
+        </is>
+      </c>
+      <c r="E12" t="inlineStr">
+        <is>
+          <t>4</t>
+        </is>
+      </c>
+      <c r="G12" t="inlineStr">
+        <is>
+          <t>46</t>
+        </is>
+      </c>
+      <c r="H12" t="inlineStr">
+        <is>
+          <t>38</t>
+        </is>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="inlineStr">
+        <is>
+          <t>PTSW1_Floor7</t>
+        </is>
+      </c>
+      <c r="B13" t="inlineStr">
+        <is>
+          <t>JUNOS Base OS boot [12.3R12.4]</t>
+        </is>
+      </c>
+      <c r="C13" t="inlineStr">
+        <is>
+          <t>ex3300-48p</t>
+        </is>
+      </c>
+      <c r="D13" t="inlineStr">
+        <is>
+          <t>10.9.106.37/23</t>
+        </is>
+      </c>
+      <c r="E13" t="inlineStr">
+        <is>
+          <t>4</t>
+        </is>
+      </c>
+      <c r="G13" t="inlineStr">
+        <is>
+          <t>72</t>
+        </is>
+      </c>
+      <c r="H13" t="inlineStr">
+        <is>
+          <t>39</t>
+        </is>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="inlineStr">
+        <is>
+          <t>floor7_sw_lab</t>
+        </is>
+      </c>
+      <c r="B14" t="inlineStr">
+        <is>
+          <t>JUNOS Base OS boot [12.3R12.4]</t>
+        </is>
+      </c>
+      <c r="C14" t="inlineStr">
+        <is>
+          <t>ex3300-24p</t>
+        </is>
+      </c>
+      <c r="D14" t="inlineStr">
+        <is>
+          <t>10.9.106.30/23</t>
+        </is>
+      </c>
+      <c r="E14" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="G14" t="inlineStr">
+        <is>
+          <t>4</t>
+        </is>
+      </c>
+      <c r="H14" t="inlineStr">
+        <is>
+          <t>34</t>
+        </is>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="inlineStr">
+        <is>
+          <t>PTSW2_Floor7</t>
+        </is>
+      </c>
+      <c r="B15" t="inlineStr">
+        <is>
+          <t>JUNOS Base OS boot [12.3R12.4]</t>
+        </is>
+      </c>
+      <c r="C15" t="inlineStr">
+        <is>
+          <t>ex3300-48p</t>
+        </is>
+      </c>
+      <c r="D15" t="inlineStr">
+        <is>
+          <t>10.9.106.38/23</t>
+        </is>
+      </c>
+      <c r="E15" t="inlineStr">
+        <is>
+          <t>4</t>
+        </is>
+      </c>
+      <c r="G15" t="inlineStr">
+        <is>
+          <t>70</t>
+        </is>
+      </c>
+      <c r="H15" t="inlineStr">
+        <is>
+          <t>38</t>
+        </is>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="inlineStr">
+        <is>
+          <t>PTSW1_Floor7</t>
+        </is>
+      </c>
+      <c r="B16" t="inlineStr">
+        <is>
+          <t>JUNOS Base OS boot [12.3R12.4]</t>
+        </is>
+      </c>
+      <c r="C16" t="inlineStr">
+        <is>
+          <t>ex3300-48p</t>
+        </is>
+      </c>
+      <c r="D16" t="inlineStr">
+        <is>
+          <t>10.9.106.37/23</t>
+        </is>
+      </c>
+      <c r="E16" t="inlineStr">
+        <is>
+          <t>4</t>
+        </is>
+      </c>
+      <c r="G16" t="inlineStr">
+        <is>
+          <t>68</t>
+        </is>
+      </c>
+      <c r="H16" t="inlineStr">
+        <is>
+          <t>39</t>
+        </is>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="inlineStr">
+        <is>
+          <t>PTSW1_Floor7</t>
+        </is>
+      </c>
+      <c r="B17" t="inlineStr">
+        <is>
+          <t>JUNOS Base OS boot [12.3R12.4]</t>
+        </is>
+      </c>
+      <c r="C17" t="inlineStr">
+        <is>
+          <t>ex3300-48p</t>
+        </is>
+      </c>
+      <c r="D17" t="inlineStr">
+        <is>
+          <t>10.9.106.37/23</t>
+        </is>
+      </c>
+      <c r="E17" t="inlineStr">
+        <is>
+          <t>4</t>
+        </is>
+      </c>
+      <c r="G17" t="inlineStr">
+        <is>
+          <t>58</t>
+        </is>
+      </c>
+      <c r="H17" t="inlineStr">
+        <is>
+          <t>39</t>
+        </is>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="inlineStr">
+        <is>
+          <t>floor7_sw_lab</t>
+        </is>
+      </c>
+      <c r="B18" t="inlineStr">
+        <is>
+          <t>JUNOS Base OS boot [12.3R12.4]</t>
+        </is>
+      </c>
+      <c r="C18" t="inlineStr">
+        <is>
+          <t>ex3300-24p</t>
+        </is>
+      </c>
+      <c r="D18" t="inlineStr">
+        <is>
+          <t>10.9.106.30/23</t>
+        </is>
+      </c>
+      <c r="E18" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="G18" t="inlineStr">
+        <is>
+          <t>5</t>
+        </is>
+      </c>
+      <c r="H18" t="inlineStr">
+        <is>
+          <t>34</t>
+        </is>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" t="inlineStr">
+        <is>
+          <t>floor7_sw_lab</t>
+        </is>
+      </c>
+      <c r="B19" t="inlineStr">
+        <is>
+          <t>JUNOS Base OS boot [12.3R12.4]</t>
+        </is>
+      </c>
+      <c r="C19" t="inlineStr">
+        <is>
+          <t>ex3300-24p</t>
+        </is>
+      </c>
+      <c r="D19" t="inlineStr">
+        <is>
+          <t>10.9.106.30/23</t>
+        </is>
+      </c>
+      <c r="E19" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="G19" t="inlineStr">
+        <is>
+          <t>4</t>
+        </is>
+      </c>
+      <c r="H19" t="inlineStr">
+        <is>
+          <t>34</t>
+        </is>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" t="inlineStr">
+        <is>
+          <t>floor7_sw_lab</t>
+        </is>
+      </c>
+      <c r="B20" t="inlineStr">
+        <is>
+          <t>JUNOS Base OS boot [12.3R12.4]</t>
+        </is>
+      </c>
+      <c r="C20" t="inlineStr">
+        <is>
+          <t>ex3300-24p</t>
+        </is>
+      </c>
+      <c r="D20" t="inlineStr">
+        <is>
+          <t>10.9.106.30/23</t>
+        </is>
+      </c>
+      <c r="E20" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="G20" t="inlineStr">
+        <is>
+          <t>4</t>
+        </is>
+      </c>
+      <c r="H20" t="inlineStr">
+        <is>
+          <t>34</t>
+        </is>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" t="inlineStr">
+        <is>
+          <t>floor7_sw_lab</t>
+        </is>
+      </c>
+      <c r="B21" t="inlineStr">
+        <is>
+          <t>JUNOS Base OS boot [12.3R12.4]</t>
+        </is>
+      </c>
+      <c r="C21" t="inlineStr">
+        <is>
+          <t>ex3300-24p</t>
+        </is>
+      </c>
+      <c r="D21" t="inlineStr">
+        <is>
+          <t>10.9.106.30/23</t>
+        </is>
+      </c>
+      <c r="E21" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="G21" t="inlineStr">
+        <is>
+          <t>9</t>
+        </is>
+      </c>
+      <c r="H21" t="inlineStr">
+        <is>
+          <t>34</t>
+        </is>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" t="inlineStr">
+        <is>
+          <t>floor7_sw_lab</t>
+        </is>
+      </c>
+      <c r="B22" t="inlineStr">
+        <is>
+          <t>JUNOS Base OS boot [12.3R12.4]</t>
+        </is>
+      </c>
+      <c r="C22" t="inlineStr">
+        <is>
+          <t>ex3300-24p</t>
+        </is>
+      </c>
+      <c r="D22" t="inlineStr">
+        <is>
+          <t>10.9.106.30/23</t>
+        </is>
+      </c>
+      <c r="E22" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="G22" t="inlineStr">
+        <is>
+          <t>24</t>
+        </is>
+      </c>
+      <c r="H22" t="inlineStr">
+        <is>
+          <t>34</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
updated pyton savetoexcel to exept dictonary
</commit_message>
<xml_diff>
--- a/device_report.xlsx
+++ b/device_report.xlsx
@@ -1,12 +1,12 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <bookViews>
-    <workbookView activeTab="0" autoFilterDateGrouping="1" firstSheet="0" minimized="0" showHorizontalScroll="1" showSheetTabs="1" showVerticalScroll="1" tabRatio="600" visibility="visible" windowHeight="11325" windowWidth="21600" xWindow="5655" yWindow="2730"/>
+    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="5655" yWindow="2730" windowWidth="21600" windowHeight="11325" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheet" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="Sheet" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="0" fullCalcOnLoad="1"/>
@@ -56,17 +56,17 @@
     </border>
   </borders>
   <cellStyleXfs count="1">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="3">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf borderId="0" fillId="2" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle builtinId="0" name="Normal" xfId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <tableStyles count="0" defaultPivotStyle="PivotStyleLight16" defaultTableStyle="TableStyleMedium9"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
 </styleSheet>
 </file>
 
@@ -359,7 +359,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:H22"/>
+  <dimension ref="A1:H25"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="H9" sqref="H9"/>
@@ -367,11 +367,11 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <cols>
-    <col bestFit="1" customWidth="1" max="1" min="1" width="11.28515625"/>
-    <col bestFit="1" customWidth="1" max="4" min="4" width="9.140625"/>
-    <col bestFit="1" customWidth="1" max="6" min="6" width="11.7109375"/>
-    <col bestFit="1" customWidth="1" max="7" min="7" width="20.7109375"/>
-    <col bestFit="1" customWidth="1" max="8" min="8" width="24.7109375"/>
+    <col width="11.28515625" bestFit="1" customWidth="1" min="1" max="1"/>
+    <col width="9.140625" bestFit="1" customWidth="1" min="4" max="4"/>
+    <col width="11.7109375" bestFit="1" customWidth="1" min="6" max="6"/>
+    <col width="20.7109375" bestFit="1" customWidth="1" min="7" max="7"/>
+    <col width="24.7109375" bestFit="1" customWidth="1" min="8" max="8"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -1193,8 +1193,34 @@
         </is>
       </c>
     </row>
+    <row r="23">
+      <c r="A23" t="inlineStr">
+        <is>
+          <t>floor8_ptsw1</t>
+        </is>
+      </c>
+    </row>
+    <row r="24">
+      <c r="B24" t="inlineStr">
+        <is>
+          <t>192.168.0.3</t>
+        </is>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" t="inlineStr">
+        <is>
+          <t>asher1</t>
+        </is>
+      </c>
+      <c r="B25" t="inlineStr">
+        <is>
+          <t>the men1</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
-  <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
-  <pageSetup horizontalDpi="180" orientation="landscape" paperSize="261" verticalDpi="180"/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup orientation="landscape" paperSize="261" horizontalDpi="180" verticalDpi="180"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Chnaged the config to dymanic inventory and updated the excel file
</commit_message>
<xml_diff>
--- a/device_report.xlsx
+++ b/device_report.xlsx
@@ -362,7 +362,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:H16"/>
+  <dimension ref="A1:H22"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="S4" sqref="S4"/>
@@ -989,6 +989,228 @@
         </is>
       </c>
     </row>
+    <row r="17">
+      <c r="A17" t="inlineStr">
+        <is>
+          <t>floor7_sw_lab</t>
+        </is>
+      </c>
+      <c r="B17" t="inlineStr">
+        <is>
+          <t>JUNOS Base OS boot [12.3R12.4]</t>
+        </is>
+      </c>
+      <c r="C17" t="inlineStr">
+        <is>
+          <t>ex3300-24p</t>
+        </is>
+      </c>
+      <c r="D17" t="inlineStr">
+        <is>
+          <t>10.9.106.30/23</t>
+        </is>
+      </c>
+      <c r="E17" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="G17" t="inlineStr">
+        <is>
+          <t>4</t>
+        </is>
+      </c>
+      <c r="H17" t="inlineStr">
+        <is>
+          <t>34</t>
+        </is>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="inlineStr">
+        <is>
+          <t>PTSW2_Floor7</t>
+        </is>
+      </c>
+      <c r="B18" t="inlineStr">
+        <is>
+          <t>JUNOS Base OS boot [12.3R12.4]</t>
+        </is>
+      </c>
+      <c r="C18" t="inlineStr">
+        <is>
+          <t>ex3300-48p</t>
+        </is>
+      </c>
+      <c r="D18" t="inlineStr">
+        <is>
+          <t>10.9.106.38/23</t>
+        </is>
+      </c>
+      <c r="E18" t="inlineStr">
+        <is>
+          <t>4</t>
+        </is>
+      </c>
+      <c r="G18" t="inlineStr">
+        <is>
+          <t>48</t>
+        </is>
+      </c>
+      <c r="H18" t="inlineStr">
+        <is>
+          <t>38</t>
+        </is>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" t="inlineStr">
+        <is>
+          <t>PTSW1_Floor7</t>
+        </is>
+      </c>
+      <c r="B19" t="inlineStr">
+        <is>
+          <t>JUNOS Base OS boot [12.3R12.4]</t>
+        </is>
+      </c>
+      <c r="C19" t="inlineStr">
+        <is>
+          <t>ex3300-48p</t>
+        </is>
+      </c>
+      <c r="D19" t="inlineStr">
+        <is>
+          <t>10.9.106.37/23</t>
+        </is>
+      </c>
+      <c r="E19" t="inlineStr">
+        <is>
+          <t>4</t>
+        </is>
+      </c>
+      <c r="G19" t="inlineStr">
+        <is>
+          <t>73</t>
+        </is>
+      </c>
+      <c r="H19" t="inlineStr">
+        <is>
+          <t>39</t>
+        </is>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" t="inlineStr">
+        <is>
+          <t>floor7_sw_lab</t>
+        </is>
+      </c>
+      <c r="B20" t="inlineStr">
+        <is>
+          <t>JUNOS Base OS boot [12.3R12.4]</t>
+        </is>
+      </c>
+      <c r="C20" t="inlineStr">
+        <is>
+          <t>ex3300-24p</t>
+        </is>
+      </c>
+      <c r="D20" t="inlineStr">
+        <is>
+          <t>10.9.106.30/23</t>
+        </is>
+      </c>
+      <c r="E20" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="G20" t="inlineStr">
+        <is>
+          <t>4</t>
+        </is>
+      </c>
+      <c r="H20" t="inlineStr">
+        <is>
+          <t>34</t>
+        </is>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" t="inlineStr">
+        <is>
+          <t>PTSW1_Floor7</t>
+        </is>
+      </c>
+      <c r="B21" t="inlineStr">
+        <is>
+          <t>JUNOS Base OS boot [12.3R12.4]</t>
+        </is>
+      </c>
+      <c r="C21" t="inlineStr">
+        <is>
+          <t>ex3300-48p</t>
+        </is>
+      </c>
+      <c r="D21" t="inlineStr">
+        <is>
+          <t>10.9.106.37/23</t>
+        </is>
+      </c>
+      <c r="E21" t="inlineStr">
+        <is>
+          <t>4</t>
+        </is>
+      </c>
+      <c r="G21" t="inlineStr">
+        <is>
+          <t>69</t>
+        </is>
+      </c>
+      <c r="H21" t="inlineStr">
+        <is>
+          <t>39</t>
+        </is>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" t="inlineStr">
+        <is>
+          <t>PTSW2_Floor7</t>
+        </is>
+      </c>
+      <c r="B22" t="inlineStr">
+        <is>
+          <t>JUNOS Base OS boot [12.3R12.4]</t>
+        </is>
+      </c>
+      <c r="C22" t="inlineStr">
+        <is>
+          <t>ex3300-48p</t>
+        </is>
+      </c>
+      <c r="D22" t="inlineStr">
+        <is>
+          <t>10.9.106.38/23</t>
+        </is>
+      </c>
+      <c r="E22" t="inlineStr">
+        <is>
+          <t>4</t>
+        </is>
+      </c>
+      <c r="G22" t="inlineStr">
+        <is>
+          <t>73</t>
+        </is>
+      </c>
+      <c r="H22" t="inlineStr">
+        <is>
+          <t>38</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
   <pageSetup horizontalDpi="180" orientation="landscape" paperSize="261" verticalDpi="180"/>

</xml_diff>

<commit_message>
Create group var for ex3400 switches
</commit_message>
<xml_diff>
--- a/device_report.xlsx
+++ b/device_report.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <bookViews>
-    <workbookView activeTab="0" autoFilterDateGrouping="1" firstSheet="0" minimized="0" showHorizontalScroll="1" showSheetTabs="1" showVerticalScroll="1" tabRatio="600" visibility="visible" windowHeight="15840" windowWidth="29040" xWindow="28680" yWindow="-120"/>
+    <workbookView activeTab="0" autoFilterDateGrouping="1" firstSheet="0" minimized="0" showHorizontalScroll="1" showSheetTabs="1" showVerticalScroll="1" tabRatio="600" visibility="visible" windowHeight="11385" windowWidth="21600" xWindow="3975" yWindow="1695"/>
   </bookViews>
   <sheets>
     <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
@@ -364,10 +364,10 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G10"/>
+  <dimension ref="A1:G4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G11" sqref="G11"/>
+      <selection activeCell="G2" sqref="A2:G10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
@@ -442,12 +442,12 @@
       </c>
       <c r="F2" t="inlineStr">
         <is>
-          <t>4</t>
+          <t>40</t>
         </is>
       </c>
       <c r="G2" t="inlineStr">
         <is>
-          <t>35</t>
+          <t>34</t>
         </is>
       </c>
     </row>
@@ -479,7 +479,7 @@
       </c>
       <c r="F3" t="inlineStr">
         <is>
-          <t>66</t>
+          <t>69</t>
         </is>
       </c>
       <c r="G3" t="inlineStr">
@@ -516,232 +516,10 @@
       </c>
       <c r="F4" t="inlineStr">
         <is>
-          <t>72</t>
+          <t>31</t>
         </is>
       </c>
       <c r="G4" t="inlineStr">
-        <is>
-          <t>38</t>
-        </is>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5" t="inlineStr">
-        <is>
-          <t>floor7_sw_lab</t>
-        </is>
-      </c>
-      <c r="B5" t="inlineStr">
-        <is>
-          <t>JUNOS Base OS boot [12.3R12.4]</t>
-        </is>
-      </c>
-      <c r="C5" t="inlineStr">
-        <is>
-          <t>ex3300-24p</t>
-        </is>
-      </c>
-      <c r="D5" t="inlineStr">
-        <is>
-          <t>10.9.106.30/23</t>
-        </is>
-      </c>
-      <c r="E5" t="inlineStr">
-        <is>
-          <t>1</t>
-        </is>
-      </c>
-      <c r="F5" t="inlineStr">
-        <is>
-          <t>38</t>
-        </is>
-      </c>
-      <c r="G5" t="inlineStr">
-        <is>
-          <t>34</t>
-        </is>
-      </c>
-    </row>
-    <row r="6">
-      <c r="A6" t="inlineStr">
-        <is>
-          <t>PTSW1_Floor7</t>
-        </is>
-      </c>
-      <c r="B6" t="inlineStr">
-        <is>
-          <t>JUNOS Base OS boot [12.3R12.4]</t>
-        </is>
-      </c>
-      <c r="C6" t="inlineStr">
-        <is>
-          <t>ex3300-48p</t>
-        </is>
-      </c>
-      <c r="D6" t="inlineStr">
-        <is>
-          <t>10.9.106.37/23</t>
-        </is>
-      </c>
-      <c r="E6" t="inlineStr">
-        <is>
-          <t>4</t>
-        </is>
-      </c>
-      <c r="F6" t="inlineStr">
-        <is>
-          <t>66</t>
-        </is>
-      </c>
-      <c r="G6" t="inlineStr">
-        <is>
-          <t>39</t>
-        </is>
-      </c>
-    </row>
-    <row r="7">
-      <c r="A7" t="inlineStr">
-        <is>
-          <t>PTSW2_Floor7</t>
-        </is>
-      </c>
-      <c r="B7" t="inlineStr">
-        <is>
-          <t>JUNOS Base OS boot [12.3R12.4]</t>
-        </is>
-      </c>
-      <c r="C7" t="inlineStr">
-        <is>
-          <t>ex3300-48p</t>
-        </is>
-      </c>
-      <c r="D7" t="inlineStr">
-        <is>
-          <t>10.9.106.38/23</t>
-        </is>
-      </c>
-      <c r="E7" t="inlineStr">
-        <is>
-          <t>4</t>
-        </is>
-      </c>
-      <c r="F7" t="inlineStr">
-        <is>
-          <t>68</t>
-        </is>
-      </c>
-      <c r="G7" t="inlineStr">
-        <is>
-          <t>38</t>
-        </is>
-      </c>
-    </row>
-    <row r="8">
-      <c r="A8" t="inlineStr">
-        <is>
-          <t>floor7_sw_lab</t>
-        </is>
-      </c>
-      <c r="B8" t="inlineStr">
-        <is>
-          <t>JUNOS Base OS boot [12.3R12.4]</t>
-        </is>
-      </c>
-      <c r="C8" t="inlineStr">
-        <is>
-          <t>ex3300-24p</t>
-        </is>
-      </c>
-      <c r="D8" t="inlineStr">
-        <is>
-          <t>10.9.106.30/23</t>
-        </is>
-      </c>
-      <c r="E8" t="inlineStr">
-        <is>
-          <t>1</t>
-        </is>
-      </c>
-      <c r="F8" t="inlineStr">
-        <is>
-          <t>25</t>
-        </is>
-      </c>
-      <c r="G8" t="inlineStr">
-        <is>
-          <t>34</t>
-        </is>
-      </c>
-    </row>
-    <row r="9">
-      <c r="A9" t="inlineStr">
-        <is>
-          <t>PTSW1_Floor7</t>
-        </is>
-      </c>
-      <c r="B9" t="inlineStr">
-        <is>
-          <t>JUNOS Base OS boot [12.3R12.4]</t>
-        </is>
-      </c>
-      <c r="C9" t="inlineStr">
-        <is>
-          <t>ex3300-48p</t>
-        </is>
-      </c>
-      <c r="D9" t="inlineStr">
-        <is>
-          <t>10.9.106.37/23</t>
-        </is>
-      </c>
-      <c r="E9" t="inlineStr">
-        <is>
-          <t>4</t>
-        </is>
-      </c>
-      <c r="F9" t="inlineStr">
-        <is>
-          <t>68</t>
-        </is>
-      </c>
-      <c r="G9" t="inlineStr">
-        <is>
-          <t>39</t>
-        </is>
-      </c>
-    </row>
-    <row r="10">
-      <c r="A10" t="inlineStr">
-        <is>
-          <t>PTSW2_Floor7</t>
-        </is>
-      </c>
-      <c r="B10" t="inlineStr">
-        <is>
-          <t>JUNOS Base OS boot [12.3R12.4]</t>
-        </is>
-      </c>
-      <c r="C10" t="inlineStr">
-        <is>
-          <t>ex3300-48p</t>
-        </is>
-      </c>
-      <c r="D10" t="inlineStr">
-        <is>
-          <t>10.9.106.38/23</t>
-        </is>
-      </c>
-      <c r="E10" t="inlineStr">
-        <is>
-          <t>4</t>
-        </is>
-      </c>
-      <c r="F10" t="inlineStr">
-        <is>
-          <t>61</t>
-        </is>
-      </c>
-      <c r="G10" t="inlineStr">
         <is>
           <t>38</t>
         </is>

</xml_diff>

<commit_message>
added support to ex3400 switches using new task file and when tag
</commit_message>
<xml_diff>
--- a/device_report.xlsx
+++ b/device_report.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <bookViews>
-    <workbookView activeTab="0" autoFilterDateGrouping="1" firstSheet="0" minimized="0" showHorizontalScroll="1" showSheetTabs="1" showVerticalScroll="1" tabRatio="600" visibility="visible" windowHeight="11385" windowWidth="21600" xWindow="3975" yWindow="1695"/>
+    <workbookView activeTab="0" autoFilterDateGrouping="1" firstSheet="0" minimized="0" showHorizontalScroll="1" showSheetTabs="1" showVerticalScroll="1" tabRatio="600" visibility="visible" windowHeight="11385" windowWidth="21600" xWindow="5010" yWindow="2730"/>
   </bookViews>
   <sheets>
     <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
@@ -364,10 +364,10 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G4"/>
+  <dimension ref="A1:G5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G2" sqref="A2:G10"/>
+      <selection activeCell="A2" sqref="A2:G14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
@@ -442,7 +442,7 @@
       </c>
       <c r="F2" t="inlineStr">
         <is>
-          <t>40</t>
+          <t>28</t>
         </is>
       </c>
       <c r="G2" t="inlineStr">
@@ -516,12 +516,49 @@
       </c>
       <c r="F4" t="inlineStr">
         <is>
-          <t>31</t>
+          <t>61</t>
         </is>
       </c>
       <c r="G4" t="inlineStr">
         <is>
-          <t>38</t>
+          <t>39</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>oren-flr1sw-B1</t>
+        </is>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>JUNOS OS Kernel 32-bit  [20180119.e26d166_builder_master]</t>
+        </is>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>ex3400-48p</t>
+        </is>
+      </c>
+      <c r="D5" t="inlineStr">
+        <is>
+          <t>10.9.106.11/23</t>
+        </is>
+      </c>
+      <c r="E5" t="inlineStr">
+        <is>
+          <t>4</t>
+        </is>
+      </c>
+      <c r="F5" t="inlineStr">
+        <is>
+          <t>23</t>
+        </is>
+      </c>
+      <c r="G5" t="inlineStr">
+        <is>
+          <t>18</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Add support to ex2300 switch
</commit_message>
<xml_diff>
--- a/device_report.xlsx
+++ b/device_report.xlsx
@@ -364,7 +364,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G5"/>
+  <dimension ref="A1:G9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="A2" sqref="A2:G14"/>
@@ -562,6 +562,154 @@
         </is>
       </c>
     </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>floor7_sw_lab</t>
+        </is>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>JUNOS Base OS boot [12.3R12.4]</t>
+        </is>
+      </c>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>ex3300-24p</t>
+        </is>
+      </c>
+      <c r="D6" t="inlineStr">
+        <is>
+          <t>10.9.106.30/23</t>
+        </is>
+      </c>
+      <c r="E6" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="F6" t="inlineStr">
+        <is>
+          <t>38</t>
+        </is>
+      </c>
+      <c r="G6" t="inlineStr">
+        <is>
+          <t>34</t>
+        </is>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>PTSW1_Floor7</t>
+        </is>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>JUNOS Base OS boot [12.3R12.4]</t>
+        </is>
+      </c>
+      <c r="C7" t="inlineStr">
+        <is>
+          <t>ex3300-48p</t>
+        </is>
+      </c>
+      <c r="D7" t="inlineStr">
+        <is>
+          <t>10.9.106.37/23</t>
+        </is>
+      </c>
+      <c r="E7" t="inlineStr">
+        <is>
+          <t>4</t>
+        </is>
+      </c>
+      <c r="F7" t="inlineStr">
+        <is>
+          <t>66</t>
+        </is>
+      </c>
+      <c r="G7" t="inlineStr">
+        <is>
+          <t>39</t>
+        </is>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>PTSW2_Floor7</t>
+        </is>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>JUNOS Base OS boot [12.3R12.4]</t>
+        </is>
+      </c>
+      <c r="C8" t="inlineStr">
+        <is>
+          <t>ex3300-48p</t>
+        </is>
+      </c>
+      <c r="D8" t="inlineStr">
+        <is>
+          <t>10.9.106.38/23</t>
+        </is>
+      </c>
+      <c r="E8" t="inlineStr">
+        <is>
+          <t>4</t>
+        </is>
+      </c>
+      <c r="F8" t="inlineStr">
+        <is>
+          <t>71</t>
+        </is>
+      </c>
+      <c r="G8" t="inlineStr">
+        <is>
+          <t>38</t>
+        </is>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>oren-flr1sw-B1</t>
+        </is>
+      </c>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>JUNOS OS Kernel 32-bit  [20180119.e26d166_builder_master]</t>
+        </is>
+      </c>
+      <c r="C9" t="inlineStr">
+        <is>
+          <t>ex3400-48p</t>
+        </is>
+      </c>
+      <c r="D9" t="inlineStr">
+        <is>
+          <t>10.9.106.11/23</t>
+        </is>
+      </c>
+      <c r="E9" t="inlineStr">
+        <is>
+          <t>4</t>
+        </is>
+      </c>
+      <c r="F9" t="inlineStr">
+        <is>
+          <t>32</t>
+        </is>
+      </c>
+      <c r="G9" t="inlineStr">
+        <is>
+          <t>17</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>

</xml_diff>

<commit_message>
Add task that handels with general device type
</commit_message>
<xml_diff>
--- a/device_report.xlsx
+++ b/device_report.xlsx
@@ -364,7 +364,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G9"/>
+  <dimension ref="A1:G19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="A2" sqref="A2:G14"/>
@@ -710,6 +710,276 @@
         </is>
       </c>
     </row>
+    <row r="10">
+      <c r="A10" t="inlineStr">
+        <is>
+          <t>pt-router-guest</t>
+        </is>
+      </c>
+      <c r="B10" t="inlineStr">
+        <is>
+          <t>JUNOS Software Release [15.1X49-D170.4]</t>
+        </is>
+      </c>
+      <c r="C10" t="inlineStr">
+        <is>
+          <t>srx300</t>
+        </is>
+      </c>
+      <c r="F10" t="inlineStr">
+        <is>
+          <t>34</t>
+        </is>
+      </c>
+      <c r="G10" t="inlineStr">
+        <is>
+          <t>28</t>
+        </is>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="inlineStr">
+        <is>
+          <t>pt-router-guest</t>
+        </is>
+      </c>
+      <c r="B11" t="inlineStr">
+        <is>
+          <t>JUNOS Software Release [15.1X49-D170.4]</t>
+        </is>
+      </c>
+      <c r="C11" t="inlineStr">
+        <is>
+          <t>srx300</t>
+        </is>
+      </c>
+      <c r="F11" t="inlineStr">
+        <is>
+          <t>25</t>
+        </is>
+      </c>
+      <c r="G11" t="inlineStr">
+        <is>
+          <t>28</t>
+        </is>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="inlineStr">
+        <is>
+          <t>pt-router-guest</t>
+        </is>
+      </c>
+      <c r="B12" t="inlineStr">
+        <is>
+          <t>JUNOS Software Release [15.1X49-D170.4]</t>
+        </is>
+      </c>
+      <c r="C12" t="inlineStr">
+        <is>
+          <t>srx300</t>
+        </is>
+      </c>
+      <c r="F12" t="inlineStr">
+        <is>
+          <t>30</t>
+        </is>
+      </c>
+      <c r="G12" t="inlineStr">
+        <is>
+          <t>28</t>
+        </is>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="inlineStr">
+        <is>
+          <t>pt-router-guest</t>
+        </is>
+      </c>
+      <c r="B13" t="inlineStr">
+        <is>
+          <t>JUNOS Software Release [15.1X49-D170.4]</t>
+        </is>
+      </c>
+      <c r="C13" t="inlineStr">
+        <is>
+          <t>srx300</t>
+        </is>
+      </c>
+      <c r="F13" t="inlineStr">
+        <is>
+          <t>28</t>
+        </is>
+      </c>
+      <c r="G13" t="inlineStr">
+        <is>
+          <t>28</t>
+        </is>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="inlineStr">
+        <is>
+          <t>pt-router-guest</t>
+        </is>
+      </c>
+      <c r="B14" t="inlineStr">
+        <is>
+          <t>JUNOS Software Release [15.1X49-D170.4]</t>
+        </is>
+      </c>
+      <c r="C14" t="inlineStr">
+        <is>
+          <t>srx300</t>
+        </is>
+      </c>
+      <c r="F14" t="inlineStr">
+        <is>
+          <t>34</t>
+        </is>
+      </c>
+      <c r="G14" t="inlineStr">
+        <is>
+          <t>28</t>
+        </is>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="inlineStr">
+        <is>
+          <t>pt-router-guest</t>
+        </is>
+      </c>
+      <c r="B15" t="inlineStr">
+        <is>
+          <t>JUNOS Software Release [15.1X49-D170.4]</t>
+        </is>
+      </c>
+      <c r="C15" t="inlineStr">
+        <is>
+          <t>srx300</t>
+        </is>
+      </c>
+      <c r="F15" t="inlineStr">
+        <is>
+          <t>30</t>
+        </is>
+      </c>
+      <c r="G15" t="inlineStr">
+        <is>
+          <t>28</t>
+        </is>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="inlineStr">
+        <is>
+          <t>pt-router-guest</t>
+        </is>
+      </c>
+      <c r="B16" t="inlineStr">
+        <is>
+          <t>JUNOS Software Release [15.1X49-D170.4]</t>
+        </is>
+      </c>
+      <c r="C16" t="inlineStr">
+        <is>
+          <t>srx300</t>
+        </is>
+      </c>
+      <c r="F16" t="inlineStr">
+        <is>
+          <t>32</t>
+        </is>
+      </c>
+      <c r="G16" t="inlineStr">
+        <is>
+          <t>28</t>
+        </is>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="inlineStr">
+        <is>
+          <t>pt-router-guest</t>
+        </is>
+      </c>
+      <c r="B17" t="inlineStr">
+        <is>
+          <t>JUNOS Software Release [15.1X49-D170.4]</t>
+        </is>
+      </c>
+      <c r="C17" t="inlineStr">
+        <is>
+          <t>srx300</t>
+        </is>
+      </c>
+      <c r="F17" t="inlineStr">
+        <is>
+          <t>24</t>
+        </is>
+      </c>
+      <c r="G17" t="inlineStr">
+        <is>
+          <t>28</t>
+        </is>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="inlineStr">
+        <is>
+          <t>pt-router-ext1</t>
+        </is>
+      </c>
+      <c r="B18" t="inlineStr">
+        <is>
+          <t>17.4R2.4</t>
+        </is>
+      </c>
+      <c r="C18" t="inlineStr">
+        <is>
+          <t>mx204</t>
+        </is>
+      </c>
+      <c r="F18" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="G18" t="inlineStr">
+        <is>
+          <t>10</t>
+        </is>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" t="inlineStr">
+        <is>
+          <t>pt-router-ext1</t>
+        </is>
+      </c>
+      <c r="B19" t="inlineStr">
+        <is>
+          <t>17.4R2.4</t>
+        </is>
+      </c>
+      <c r="C19" t="inlineStr">
+        <is>
+          <t>mx204</t>
+        </is>
+      </c>
+      <c r="F19" t="inlineStr">
+        <is>
+          <t>5</t>
+        </is>
+      </c>
+      <c r="G19" t="inlineStr">
+        <is>
+          <t>10</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>

</xml_diff>